<commit_message>
update sa of 20210510
</commit_message>
<xml_diff>
--- a/TagSeq/Analysis/Output/MS_materials/Tables/KEGG_WGCNA_summary.xlsx
+++ b/TagSeq/Analysis/Output/MS_materials/Tables/KEGG_WGCNA_summary.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjg\Documents\My_Projects\Pgenerosa_TagSeq_Metabolomics\TagSeq\Analysis\Output\MS_materials\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F229DE9-96A6-483A-96C9-194C923F51BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C08E55-6EEA-41F9-96F3-16EFA07DB2ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{10F09BC0-F421-4E18-B283-2FBE16DB1E0F}"/>
+    <workbookView xWindow="-28920" yWindow="-10305" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{10F09BC0-F421-4E18-B283-2FBE16DB1E0F}"/>
   </bookViews>
   <sheets>
-    <sheet name="top_Pvals" sheetId="1" r:id="rId1"/>
-    <sheet name="allPvals" sheetId="2" r:id="rId2"/>
+    <sheet name="DESeq2_MainEffects" sheetId="4" r:id="rId1"/>
+    <sheet name="WGCNA_all_genes" sheetId="3" r:id="rId2"/>
+    <sheet name="WGCNA_MF_GOseq_NOTUSED" sheetId="1" r:id="rId3"/>
+    <sheet name="WGCNA_BP_GOseq_NOTUSED" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="179">
   <si>
     <t>Day7</t>
   </si>
@@ -585,6 +587,318 @@
   <si>
     <t>65 ± 9</t>
   </si>
+  <si>
+    <t>10 of 108</t>
+  </si>
+  <si>
+    <t>16 of 108</t>
+  </si>
+  <si>
+    <t>7 of 108</t>
+  </si>
+  <si>
+    <t>9 of 108</t>
+  </si>
+  <si>
+    <t>4 of 108</t>
+  </si>
+  <si>
+    <t>BgRatio</t>
+  </si>
+  <si>
+    <t>40/3837</t>
+  </si>
+  <si>
+    <t>191/3837</t>
+  </si>
+  <si>
+    <t>96/3837</t>
+  </si>
+  <si>
+    <t>59/3837</t>
+  </si>
+  <si>
+    <t>110/3837</t>
+  </si>
+  <si>
+    <t>23/3837</t>
+  </si>
+  <si>
+    <t>10 of 56</t>
+  </si>
+  <si>
+    <t>177/3837</t>
+  </si>
+  <si>
+    <t>17 of 164</t>
+  </si>
+  <si>
+    <t>11 of 164</t>
+  </si>
+  <si>
+    <t>12 of 164</t>
+  </si>
+  <si>
+    <t>21 of 164</t>
+  </si>
+  <si>
+    <t>6 of 164</t>
+  </si>
+  <si>
+    <t>30/3837</t>
+  </si>
+  <si>
+    <t>Proteasome</t>
+  </si>
+  <si>
+    <t>45/3837</t>
+  </si>
+  <si>
+    <t>5 of 61</t>
+  </si>
+  <si>
+    <t>140/3837</t>
+  </si>
+  <si>
+    <t>6 of 21</t>
+  </si>
+  <si>
+    <t>12 of 182</t>
+  </si>
+  <si>
+    <t>21 of 182</t>
+  </si>
+  <si>
+    <t>13 of 182</t>
+  </si>
+  <si>
+    <t>6 of 182</t>
+  </si>
+  <si>
+    <t>19 of 182</t>
+  </si>
+  <si>
+    <t>Protein processing in endoplasmic reticulum</t>
+  </si>
+  <si>
+    <t>8 of 34</t>
+  </si>
+  <si>
+    <t>141/3837</t>
+  </si>
+  <si>
+    <t>4 of 34</t>
+  </si>
+  <si>
+    <t>66/3837</t>
+  </si>
+  <si>
+    <t>7 of 78</t>
+  </si>
+  <si>
+    <t>55/3837</t>
+  </si>
+  <si>
+    <t>12 of 107</t>
+  </si>
+  <si>
+    <t>79/3837</t>
+  </si>
+  <si>
+    <t>16 of 107</t>
+  </si>
+  <si>
+    <t>144/3837</t>
+  </si>
+  <si>
+    <t>14 of 107</t>
+  </si>
+  <si>
+    <t>11 of 107</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">%  mapped to </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>C. gigas</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>p-value</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>adj</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Total genes module</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+  </si>
+  <si>
+    <t>DESeq2 Main pairwise effects</t>
+  </si>
+  <si>
+    <r>
+      <t>Total genes effect</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+  </si>
+  <si>
+    <t>A × M</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary </t>
+  </si>
+  <si>
+    <t>tretament</t>
+  </si>
+  <si>
+    <t>pairwise effect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">downregulated </t>
+  </si>
+  <si>
+    <t>upregulated</t>
+  </si>
+  <si>
+    <r>
+      <t>62</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (40)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>46</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (17)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">54 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(26)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">101 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(56)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">112 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(64)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>317</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (212)</t>
+    </r>
+  </si>
+  <si>
+    <t>7 of 22</t>
+  </si>
+  <si>
+    <t>63 ± 5</t>
+  </si>
+  <si>
+    <t>%  mapped</t>
+  </si>
 </sst>
 </file>
 
@@ -594,7 +908,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -655,6 +969,54 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -664,7 +1026,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -708,11 +1070,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -796,6 +1167,25 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1109,11 +1499,1511 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E3EFED-F52E-4EF0-A9C8-F55B849E4E9E}">
+  <dimension ref="B2:K29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13" style="1" customWidth="1"/>
+    <col min="4" max="5" width="17.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" style="1" customWidth="1"/>
+    <col min="8" max="10" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="42.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="1.42578125" style="1" customWidth="1"/>
+    <col min="13" max="17" width="9.140625" style="1"/>
+    <col min="18" max="18" width="14.85546875" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+    </row>
+    <row r="3" spans="2:11" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+    </row>
+    <row r="5" spans="2:11" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="G5" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+    </row>
+    <row r="6" spans="2:11" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="E6" s="42"/>
+      <c r="F6" s="47" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6" s="45" t="s">
+        <v>158</v>
+      </c>
+      <c r="H6" s="45" t="s">
+        <v>159</v>
+      </c>
+      <c r="I6" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="K6" s="43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" s="8" customFormat="1" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+    </row>
+    <row r="8" spans="2:11" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="2:11" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="G9" s="10">
+        <v>80</v>
+      </c>
+      <c r="H9" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" s="8" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+    </row>
+    <row r="11" spans="2:11" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="G11" s="10">
+        <v>52.9</v>
+      </c>
+      <c r="H11" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+    </row>
+    <row r="13" spans="2:11" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+    </row>
+    <row r="14" spans="2:11" s="8" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+    </row>
+    <row r="15" spans="2:11" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+    </row>
+    <row r="16" spans="2:11" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+    </row>
+    <row r="17" spans="2:11" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+    </row>
+    <row r="18" spans="2:11" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="G18" s="10">
+        <v>57.1</v>
+      </c>
+      <c r="H18" s="15">
+        <v>1E-3</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="K18" s="15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" s="8" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+    </row>
+    <row r="20" spans="2:11" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="G20" s="10">
+        <v>60.9</v>
+      </c>
+      <c r="H20" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+    </row>
+    <row r="22" spans="2:11" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+    </row>
+    <row r="23" spans="2:11" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="G23" s="10">
+        <v>60.7</v>
+      </c>
+      <c r="H23" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="K23" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" s="8" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+    </row>
+    <row r="25" spans="2:11" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="G25" s="10">
+        <v>53.8</v>
+      </c>
+      <c r="H25" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="K25" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+    </row>
+    <row r="27" spans="2:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="13"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+    </row>
+    <row r="28" spans="2:11" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
+    </row>
+    <row r="29" spans="2:11" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{971CC544-8200-4B40-9F8B-647C368E410B}">
+  <dimension ref="B2:I60"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="1" customWidth="1"/>
+    <col min="6" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="41.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="1.42578125" style="1" customWidth="1"/>
+    <col min="11" max="15" width="9.140625" style="1"/>
+    <col min="16" max="16" width="14.85546875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+    </row>
+    <row r="3" spans="2:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+    </row>
+    <row r="5" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E5" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+    </row>
+    <row r="6" spans="2:9" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="F6" s="45" t="s">
+        <v>159</v>
+      </c>
+      <c r="G6" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6" s="43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" s="8" customFormat="1" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+    </row>
+    <row r="8" spans="2:9" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="10">
+        <v>60.9</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="17">
+        <v>2.6850550476955398E-3</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="17">
+        <v>8.1444356826223495E-3</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="17">
+        <v>2.3517411311285499E-2</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="17">
+        <v>4.63741307300242E-2</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="17">
+        <v>4.63741307300242E-2</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+    </row>
+    <row r="16" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="10">
+        <v>61.5</v>
+      </c>
+      <c r="F16" s="17">
+        <v>1.04316759070001E-2</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+    </row>
+    <row r="18" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" s="10">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="F18" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+    </row>
+    <row r="20" spans="2:9" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+    </row>
+    <row r="21" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" s="10">
+        <v>62.2</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="17">
+        <v>7.27260969107883E-4</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="17">
+        <v>1.84994195133312E-2</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="I26" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+    </row>
+    <row r="28" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E28" s="10">
+        <v>60.5</v>
+      </c>
+      <c r="F28" s="17">
+        <v>4.5793268469314002E-2</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="I28" s="15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+    </row>
+    <row r="30" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E30" s="10">
+        <v>61.3</v>
+      </c>
+      <c r="F30" s="17">
+        <v>1.17034196947984E-3</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="H30" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="I30" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+    </row>
+    <row r="32" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="4"/>
+      <c r="C32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32" s="10">
+        <v>61.9</v>
+      </c>
+      <c r="F32" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I32" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+    </row>
+    <row r="34" spans="2:9" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+    </row>
+    <row r="35" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E35" s="10">
+        <v>61.7</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G35" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="H35" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="I35" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="17">
+        <v>6.8466012588817404E-4</v>
+      </c>
+      <c r="G36" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="H36" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="I36" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="17">
+        <v>6.7877667413907697E-3</v>
+      </c>
+      <c r="G37" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="H37" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="I37" s="15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="17">
+        <v>9.3522007181930794E-3</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="I38" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="17">
+        <v>9.3522007181930794E-3</v>
+      </c>
+      <c r="G39" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="H39" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="I39" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="17">
+        <v>9.3522007181930794E-3</v>
+      </c>
+      <c r="G40" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="H40" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="I40" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+    </row>
+    <row r="42" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="4"/>
+      <c r="C42" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="E42" s="10">
+        <v>65.8</v>
+      </c>
+      <c r="F42" s="17">
+        <v>7.2679564817444795E-4</v>
+      </c>
+      <c r="G42" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="I42" s="15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="17">
+        <v>4.1460508094533499E-2</v>
+      </c>
+      <c r="G43" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H43" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="I43" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
+    </row>
+    <row r="45" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="4"/>
+      <c r="C45" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E45" s="10">
+        <v>58.7</v>
+      </c>
+      <c r="F45" s="17">
+        <v>6.7866829875082796E-3</v>
+      </c>
+      <c r="G45" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="I45" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+    </row>
+    <row r="47" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="4"/>
+      <c r="C47" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E47" s="10">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G47" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="H47" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I47" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G48" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="H48" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="I48" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="17">
+        <v>5.1855025257350204E-4</v>
+      </c>
+      <c r="G49" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="H49" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="I49" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="17">
+        <v>2.55144760094701E-2</v>
+      </c>
+      <c r="G50" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="H50" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="I50" s="15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
+    </row>
+    <row r="52" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="4"/>
+      <c r="C52" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E52" s="10">
+        <v>53.7</v>
+      </c>
+      <c r="F52" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G52" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H52" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I52" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+    </row>
+    <row r="54" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="4"/>
+      <c r="C54" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E54" s="10">
+        <v>70.3</v>
+      </c>
+      <c r="F54" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G54" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H54" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I54" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="34"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+    </row>
+    <row r="56" spans="2:9" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="4"/>
+      <c r="C56" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E56" s="10">
+        <v>62.3</v>
+      </c>
+      <c r="F56" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G56" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H56" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I56" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" s="8" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+    </row>
+    <row r="58" spans="2:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+    </row>
+    <row r="59" spans="2:9" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="27"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="27"/>
+      <c r="E59" s="27"/>
+      <c r="F59" s="27"/>
+      <c r="G59" s="27"/>
+      <c r="H59" s="27"/>
+      <c r="I59" s="27"/>
+    </row>
+    <row r="60" spans="2:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EDB6705-7FEC-4F79-8423-266102861C73}">
   <dimension ref="B2:I52"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31:E32"/>
+      <selection activeCell="F37" sqref="F37:F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2094,12 +3984,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EA4A366-0E85-4F0D-98A9-5E1A5E006EC2}">
   <dimension ref="B2:O84"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I12" sqref="G12:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>